<commit_message>
use excel file for review
</commit_message>
<xml_diff>
--- a/src/data/FAQ_JOHN_REVIEW.xlsx
+++ b/src/data/FAQ_JOHN_REVIEW.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jshen/workspace/wits-faq-bot/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D260A1A-8D91-5044-BFB9-025672C74E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D27F5FE3-03BB-214C-B6F6-9987E5BE496B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4660" yWindow="1380" windowWidth="35980" windowHeight="20060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="230323" sheetId="14" r:id="rId1"/>
@@ -22,17 +22,28 @@
     <definedName name="Q如何申請喪葬奠儀" localSheetId="0">'230323'!$C$170</definedName>
     <definedName name="Q如何申請生育賀儀" localSheetId="0">'230323'!$C$172</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1345" uniqueCount="743">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1349" uniqueCount="745">
   <si>
     <t>Finance</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -3112,6 +3123,12 @@
   </si>
   <si>
     <t>有的，https://faq.wistronits.com/redmine</t>
+  </si>
+  <si>
+    <t>緯創軟體公司電話</t>
+  </si>
+  <si>
+    <t>886-2-7745-8888</t>
   </si>
 </sst>
 </file>
@@ -3761,11 +3778,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I220"/>
+  <dimension ref="A1:I221"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="143" zoomScaleNormal="87" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A215" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D223" sqref="D223"/>
+      <pane ySplit="1" topLeftCell="A212" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D215" sqref="D215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="18"/>
@@ -8864,6 +8881,20 @@
       </c>
       <c r="D220" s="6" t="s">
         <v>742</v>
+      </c>
+    </row>
+    <row r="221" spans="1:9">
+      <c r="A221" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="B221" s="2" t="s">
+        <v>740</v>
+      </c>
+      <c r="C221" s="2" t="s">
+        <v>743</v>
+      </c>
+      <c r="D221" s="3" t="s">
+        <v>744</v>
       </c>
     </row>
   </sheetData>

</xml_diff>